<commit_message>
Altering gem name to conform to Ruby conventions (all lower case). Fixing test spreadsheet so that it conforms to the MODS standard.
</commit_message>
<xml_diff>
--- a/spec/fixtures/test_002.xlsx
+++ b/spec/fixtures/test_002.xlsx
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="246">
   <si>
     <t>druid</t>
   </si>
@@ -868,9 +868,6 @@
     <t>Paris</t>
   </si>
   <si>
-    <t>iso-8601-b</t>
-  </si>
-  <si>
     <t>marcgt</t>
   </si>
   <si>
@@ -950,6 +947,9 @@
   </si>
   <si>
     <t>ti1:title</t>
+  </si>
+  <si>
+    <t>iso8601</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1203,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="282">
+  <cellStyleXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1467,6 +1467,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1638,7 +1640,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="282">
+  <cellStyles count="284">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1780,6 +1782,7 @@
     <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1920,6 +1923,7 @@
     <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2251,8 +2255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
+      <selection activeCell="DB3" sqref="DB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
@@ -2633,7 +2637,7 @@
       </c>
       <c r="DQ1" s="32"/>
       <c r="DR1" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="DS1" s="32"/>
       <c r="DT1" s="23" t="s">
@@ -2780,7 +2784,7 @@
         <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>32</v>
@@ -2857,7 +2861,7 @@
         <v>143</v>
       </c>
       <c r="AH2" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AI2" s="10" t="s">
         <v>50</v>
@@ -2882,7 +2886,7 @@
       </c>
       <c r="AP2" s="12"/>
       <c r="AQ2" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AR2" s="10" t="s">
         <v>52</v>
@@ -2907,7 +2911,7 @@
       </c>
       <c r="AY2" s="12"/>
       <c r="AZ2" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BA2" s="10" t="s">
         <v>54</v>
@@ -2932,7 +2936,7 @@
       </c>
       <c r="BH2" s="12"/>
       <c r="BI2" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="BJ2" s="10" t="s">
         <v>56</v>
@@ -3101,10 +3105,10 @@
         <v>103</v>
       </c>
       <c r="DR2" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="DS2" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="DS2" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="DT2" s="16" t="s">
         <v>84</v>
@@ -3274,7 +3278,7 @@
     </row>
     <row r="3" spans="1:186" s="38" customFormat="1" ht="45">
       <c r="B3" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" s="39"/>
       <c r="G3" s="38" t="s">
@@ -3315,12 +3319,15 @@
         <v>215</v>
       </c>
       <c r="AG3" s="40"/>
-      <c r="AH3" s="41" t="s">
-        <v>225</v>
+      <c r="AH3" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK3" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="AL3" s="43"/>
       <c r="AM3" s="41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AN3" s="41"/>
       <c r="AO3" s="41"/>
@@ -3370,11 +3377,11 @@
       </c>
       <c r="CB3" s="40"/>
       <c r="CC3" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="CD3" s="41"/>
       <c r="CE3" s="41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="CF3" s="44"/>
       <c r="CG3" s="41"/>
@@ -3390,7 +3397,7 @@
       </c>
       <c r="CT3" s="41"/>
       <c r="CU3" s="46" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
       <c r="CV3" s="47"/>
       <c r="CW3" s="42"/>
@@ -3398,38 +3405,38 @@
         <v>217</v>
       </c>
       <c r="DA3" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="DC3" s="41" t="s">
         <v>220</v>
-      </c>
-      <c r="DC3" s="41" t="s">
-        <v>221</v>
       </c>
       <c r="DD3" s="39"/>
       <c r="DG3" s="44"/>
       <c r="DH3" s="39"/>
       <c r="DK3" s="44"/>
       <c r="DL3" s="41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="DM3" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="DP3" s="39"/>
       <c r="DR3" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DT3" s="39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="DV3" s="48"/>
       <c r="DW3" s="39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="DX3" s="38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="DZ3" s="48"/>
       <c r="EA3" s="39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="ED3" s="48"/>
       <c r="EE3" s="39"/>
@@ -3437,10 +3444,10 @@
       <c r="EI3" s="39"/>
       <c r="EL3" s="48"/>
       <c r="EM3" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="EN3" s="38" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="EP3" s="39"/>
       <c r="ES3" s="49"/>
@@ -3456,16 +3463,16 @@
       <c r="FG3" s="52"/>
       <c r="FI3" s="39"/>
       <c r="FK3" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="FL3" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="FN3" s="56" t="s">
         <v>237</v>
       </c>
-      <c r="FL3" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="FN3" s="56" t="s">
-        <v>238</v>
-      </c>
       <c r="FO3" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="FQ3" s="49"/>
       <c r="FR3" s="39"/>

</xml_diff>

<commit_message>
Added missing square brackets for note type to XML template. Fixed inconsistencies in test spreadsheets so they are all the same now.
</commit_message>
<xml_diff>
--- a/spec/fixtures/test_002.xlsx
+++ b/spec/fixtures/test_002.xlsx
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="247">
   <si>
     <t>druid</t>
   </si>
@@ -949,7 +949,10 @@
     <t>ti1:title</t>
   </si>
   <si>
-    <t>iso8601</t>
+    <t>iso8601-b</t>
+  </si>
+  <si>
+    <t>1871</t>
   </si>
 </sst>
 </file>
@@ -2256,7 +2259,7 @@
   <dimension ref="A1:GD56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
-      <selection activeCell="DB3" sqref="DB3"/>
+      <selection activeCell="CS4" sqref="CS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
@@ -3392,8 +3395,8 @@
       <c r="CP3" s="40"/>
       <c r="CQ3" s="42"/>
       <c r="CR3" s="41"/>
-      <c r="CS3" s="41">
-        <v>1871</v>
+      <c r="CS3" s="41" t="s">
+        <v>246</v>
       </c>
       <c r="CT3" s="41"/>
       <c r="CU3" s="46" t="s">

</xml_diff>